<commit_message>
Minor fix in the xls report
</commit_message>
<xml_diff>
--- a/aFullReport.xlsx
+++ b/aFullReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_tpp\code-analyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D66FA09-7A69-4928-A305-979B743503F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B2851A-6A7D-439E-A57C-B8A1BD27137B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27510" yWindow="780" windowWidth="26130" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27810" yWindow="870" windowWidth="26130" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4514" uniqueCount="2054">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4513" uniqueCount="2054">
   <si>
     <t>DocumentName</t>
   </si>
@@ -6800,21 +6800,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="167">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -6848,342 +6834,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFCCCC"/>
         </patternFill>
       </fill>
@@ -7192,1000 +6842,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -8559,7 +7215,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8567,8 +7223,8 @@
     <col min="1" max="2" width="9.109375" style="8"/>
     <col min="3" max="3" width="22.44140625" customWidth="1"/>
     <col min="4" max="4" width="19.109375" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" customWidth="1"/>
+    <col min="6" max="6" width="56.6640625" customWidth="1"/>
     <col min="7" max="7" width="21.6640625" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" customWidth="1"/>
     <col min="12" max="12" width="9.109375" style="2"/>
@@ -8716,9 +7372,6 @@
       <c r="G3" t="s">
         <v>68</v>
       </c>
-      <c r="H3" t="s">
-        <v>68</v>
-      </c>
       <c r="I3" t="s">
         <v>68</v>
       </c>
@@ -54644,55 +53297,55 @@
     <sortCondition ref="C2:C930"/>
   </sortState>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="21" priority="6" stopIfTrue="1" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="10" priority="6" stopIfTrue="1" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B930">
-    <cfRule type="containsText" dxfId="20" priority="7" stopIfTrue="1" operator="containsText" text="Planned">
+    <cfRule type="containsText" dxfId="9" priority="7" stopIfTrue="1" operator="containsText" text="Planned">
       <formula>NOT(ISERROR(SEARCH("Planned",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="8" stopIfTrue="1" operator="containsText" text="In progress">
+    <cfRule type="containsText" dxfId="8" priority="8" stopIfTrue="1" operator="containsText" text="In progress">
       <formula>NOT(ISERROR(SEARCH("In progress",B2)))</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="18" priority="9">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="9">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:I1048576">
-    <cfRule type="containsBlanks" dxfId="16" priority="2">
+    <cfRule type="containsBlanks" dxfId="5" priority="2">
       <formula>LEN(TRIM(E1))=0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F999">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>$F2&lt;&gt;$H2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G999">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>$G2&lt;&gt;$I2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="J1:P1048576">
-    <cfRule type="cellIs" dxfId="15" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="12" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q1048576">
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="14" operator="between">
       <formula>1</formula>
       <formula>999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R1048576">
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="11" operator="equal">
       <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F999">
-    <cfRule type="expression" dxfId="11" priority="1">
-      <formula>$F2&lt;&gt;$H2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G999">
-    <cfRule type="expression" dxfId="12" priority="4">
-      <formula>$G2&lt;&gt;$I2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>